<commit_message>
dmgcalc works, missing custom stuff
</commit_message>
<xml_diff>
--- a/tools/dmgcalcsheet.xlsx
+++ b/tools/dmgcalcsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Projects\VSCode\Pokemonclone\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2465640-5DDE-40AE-955F-8F4B182F3A9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13412E28-2B5C-4250-9B0A-6F77B5E83F7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{8A0B4C3C-765A-46CE-9F45-BFF908B714FB}"/>
   </bookViews>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="75">
   <si>
     <t>Reference</t>
   </si>
@@ -119,12 +119,6 @@
     <t>Halfling</t>
   </si>
   <si>
-    <t>Species:</t>
-  </si>
-  <si>
-    <t>Base stats</t>
-  </si>
-  <si>
     <t>Physical power</t>
   </si>
   <si>
@@ -245,14 +239,50 @@
     <t>Reference attack for shock attacks</t>
   </si>
   <si>
-    <t>Reference attacks</t>
+    <t>Raw damage</t>
+  </si>
+  <si>
+    <t>Phys</t>
+  </si>
+  <si>
+    <t>Heat</t>
+  </si>
+  <si>
+    <t>Cold</t>
+  </si>
+  <si>
+    <t>Shock</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Species</t>
+  </si>
+  <si>
+    <t>Attacker</t>
+  </si>
+  <si>
+    <t>Defender</t>
+  </si>
+  <si>
+    <t>Attack</t>
+  </si>
+  <si>
+    <t>Power</t>
+  </si>
+  <si>
+    <t>Damage taken</t>
+  </si>
+  <si>
+    <t>Custom overrides</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -267,6 +297,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -276,7 +313,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -294,27 +331,70 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right/>
@@ -323,24 +403,29 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right/>
       <top/>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -351,50 +436,103 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="8">
     <dxf>
@@ -817,189 +955,493 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0511DE4-4E3C-4A64-A65F-7C379180ED5D}">
-  <dimension ref="B1:N17"/>
+  <dimension ref="B2:W30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="13"/>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="E6" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="5"/>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
+    <row r="2" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+    </row>
+    <row r="3" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="K3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="L3" s="4"/>
+      <c r="N3" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="O3" s="4"/>
+      <c r="Q3" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="K4" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="L4" s="10"/>
+      <c r="M4" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="N4" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="O4" s="10"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="2"/>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="12" t="str">
+        <f>VLOOKUP($K$4,Speciesdb[[Name]:[Flags]],2,0)</f>
+        <v>Humanoid</v>
+      </c>
+      <c r="M5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="2"/>
+      <c r="N5" s="19" t="str">
+        <f>VLOOKUP($N$4,Speciesdb[[Name]:[Flags]],2,0)</f>
+        <v>Humanoid</v>
+      </c>
+      <c r="O5" s="12"/>
+      <c r="T5" s="2"/>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="14">
+        <f>VLOOKUP($K$4,Speciesdb[[Name]:[Flags]],3,0)</f>
+        <v>200</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="N6" s="20">
+        <f>VLOOKUP($N$4,Speciesdb[[Name]:[Flags]],3,0)</f>
+        <v>238</v>
+      </c>
+      <c r="O6" s="14"/>
+      <c r="Q6">
+        <v>200</v>
+      </c>
+      <c r="T6" s="2"/>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" s="3" t="s">
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="14">
+        <f>VLOOKUP($K$4,Speciesdb[[Name]:[Flags]],4,0)</f>
+        <v>100</v>
+      </c>
+      <c r="M7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="N7" s="20">
+        <f>VLOOKUP($N$4,Speciesdb[[Name]:[Flags]],4,0)</f>
+        <v>60</v>
+      </c>
+      <c r="O7" s="14"/>
+      <c r="Q7">
+        <v>100</v>
+      </c>
+      <c r="T7" s="2"/>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="K8" s="13"/>
+      <c r="L8" s="14">
+        <f>VLOOKUP($K$4,Speciesdb[[Name]:[Flags]],5,0)</f>
+        <v>100</v>
+      </c>
+      <c r="M8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="N8" s="20">
+        <f>VLOOKUP($N$4,Speciesdb[[Name]:[Flags]],5,0)</f>
+        <v>115</v>
+      </c>
+      <c r="O8" s="14"/>
+      <c r="Q8">
+        <v>100</v>
+      </c>
+      <c r="T8" s="2"/>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="K9" s="13"/>
+      <c r="L9" s="14">
+        <f>VLOOKUP($K$4,Speciesdb[[Name]:[Flags]],6,0)</f>
+        <v>100</v>
+      </c>
+      <c r="M9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="N9" s="20">
+        <f>VLOOKUP($N$4,Speciesdb[[Name]:[Flags]],6,0)</f>
+        <v>80</v>
+      </c>
+      <c r="O9" s="14"/>
+      <c r="Q9">
+        <v>100</v>
+      </c>
+      <c r="T9" s="2"/>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="K10" s="13"/>
+      <c r="L10" s="14">
+        <f>VLOOKUP($K$4,Speciesdb[[Name]:[Flags]],7,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M10" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="N10" s="20">
+        <f>VLOOKUP($N$4,Speciesdb[[Name]:[Flags]],7,0)</f>
+        <v>0.3</v>
+      </c>
+      <c r="O10" s="14"/>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="T10" s="2"/>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="K11" s="13"/>
+      <c r="L11" s="14">
+        <f>VLOOKUP($K$4,Speciesdb[[Name]:[Flags]],8,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M11" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="N11" s="20">
+        <f>VLOOKUP($N$4,Speciesdb[[Name]:[Flags]],8,0)</f>
+        <v>-0.2</v>
+      </c>
+      <c r="O11" s="14"/>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="T11" s="2"/>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="K12" s="13"/>
+      <c r="L12" s="14">
+        <f>VLOOKUP($K$4,Speciesdb[[Name]:[Flags]],9,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M12" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L7" s="6" t="s">
+      <c r="N12" s="20">
+        <f>VLOOKUP($N$4,Speciesdb[[Name]:[Flags]],9,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O12" s="14"/>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="T12" s="2"/>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="K13" s="13"/>
+      <c r="L13" s="14">
+        <f>VLOOKUP($K$4,Speciesdb[[Name]:[Flags]],10,0)</f>
+        <v>100</v>
+      </c>
+      <c r="M13" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="M7" s="3" t="s">
+      <c r="N13" s="20">
+        <f>VLOOKUP($N$4,Speciesdb[[Name]:[Flags]],10,0)</f>
+        <v>80</v>
+      </c>
+      <c r="O13" s="14"/>
+      <c r="Q13">
+        <v>1</v>
+      </c>
+      <c r="T13" s="2"/>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="K14" s="13"/>
+      <c r="L14" s="14" t="str">
+        <f>VLOOKUP($K$4,Speciesdb[[Name]:[Flags]],11,0)</f>
+        <v/>
+      </c>
+      <c r="M14" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="N7" s="3" t="s">
+      <c r="N14" s="13" t="str">
+        <f>VLOOKUP($N$4,Speciesdb[[Name]:[Flags]],11,0)</f>
+        <v/>
+      </c>
+      <c r="O14" s="14"/>
+      <c r="T14" s="2"/>
+    </row>
+    <row r="15" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K15" s="15"/>
+      <c r="L15" s="16" t="str">
+        <f>VLOOKUP($K$4,Speciesdb[[Name]:[Flags]],12,0)</f>
+        <v/>
+      </c>
+      <c r="M15" s="18" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="4" t="str">
-        <f>VLOOKUP($C$2,Speciesdb!$B:$M,2)</f>
-        <v>Humanoid</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="11">
-        <f>VLOOKUP($C$2,Speciesdb!$B:$M,3)</f>
-        <v>200</v>
-      </c>
-      <c r="F8" s="7">
-        <f>VLOOKUP($C$2,Speciesdb!$B:$M,4)</f>
+      <c r="N15" s="15" t="str">
+        <f>VLOOKUP($N$4,Speciesdb[[Name]:[Flags]],12,0)</f>
+        <v/>
+      </c>
+      <c r="O15" s="16"/>
+      <c r="T15" s="2"/>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="T16" s="2"/>
+    </row>
+    <row r="17" spans="12:23" x14ac:dyDescent="0.25">
+      <c r="L17" t="s">
+        <v>71</v>
+      </c>
+      <c r="M17" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+      <c r="S17" s="2"/>
+      <c r="T17" s="2"/>
+    </row>
+    <row r="18" spans="12:23" x14ac:dyDescent="0.25">
+      <c r="L18" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="M18" t="s">
+        <v>63</v>
+      </c>
+      <c r="N18" s="24">
+        <f>VLOOKUP($M$17,Attacksdb[[Name]:[Tooltip]],2,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+    </row>
+    <row r="19" spans="12:23" x14ac:dyDescent="0.25">
+      <c r="L19" s="25"/>
+      <c r="M19" t="s">
+        <v>64</v>
+      </c>
+      <c r="N19" s="24">
+        <f>VLOOKUP($M$17,Attacksdb[[Name]:[Tooltip]],3,0)</f>
+        <v>1</v>
+      </c>
+      <c r="S19" s="2"/>
+      <c r="T19" s="2"/>
+      <c r="U19" s="2"/>
+      <c r="V19" s="2"/>
+      <c r="W19" s="2"/>
+    </row>
+    <row r="20" spans="12:23" x14ac:dyDescent="0.25">
+      <c r="L20" s="25"/>
+      <c r="M20" t="s">
+        <v>65</v>
+      </c>
+      <c r="N20" s="24">
+        <f>VLOOKUP($M$17,Attacksdb[[Name]:[Tooltip]],4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="S20" s="2"/>
+      <c r="T20" s="2"/>
+      <c r="U20" s="2"/>
+      <c r="V20" s="2"/>
+      <c r="W20" s="2"/>
+    </row>
+    <row r="21" spans="12:23" x14ac:dyDescent="0.25">
+      <c r="L21" s="25"/>
+      <c r="M21" t="s">
+        <v>66</v>
+      </c>
+      <c r="N21" s="24">
+        <f>VLOOKUP($M$17,Attacksdb[[Name]:[Tooltip]],5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="S21" s="2"/>
+      <c r="T21" s="2"/>
+      <c r="U21" s="2"/>
+      <c r="V21" s="2"/>
+      <c r="W21" s="2"/>
+    </row>
+    <row r="22" spans="12:23" x14ac:dyDescent="0.25">
+      <c r="S22" s="2"/>
+      <c r="T22" s="2"/>
+      <c r="U22" s="2"/>
+      <c r="V22" s="2"/>
+      <c r="W22" s="2"/>
+    </row>
+    <row r="23" spans="12:23" x14ac:dyDescent="0.25">
+      <c r="S23" s="2"/>
+      <c r="T23" s="2"/>
+      <c r="U23" s="2"/>
+      <c r="V23" s="2"/>
+      <c r="W23" s="2"/>
+    </row>
+    <row r="25" spans="12:23" x14ac:dyDescent="0.25">
+      <c r="L25" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="M25" s="22"/>
+      <c r="N25" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="12:23" x14ac:dyDescent="0.25">
+      <c r="L26">
+        <f>$L$7*N18</f>
+        <v>0</v>
+      </c>
+      <c r="M26" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="N26" s="26">
+        <f>L26*100/N8</f>
+        <v>0</v>
+      </c>
+      <c r="O26" s="24">
+        <f>N26/$N$6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="12:23" x14ac:dyDescent="0.25">
+      <c r="L27">
+        <f>$L$9*N19</f>
         <v>100</v>
       </c>
-      <c r="G8" s="7">
-        <f>VLOOKUP($C$2,Speciesdb!$B:$M,5)</f>
+      <c r="M27" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="N27" s="26">
+        <f>L27*(1-N10)</f>
+        <v>70</v>
+      </c>
+      <c r="O27" s="24">
+        <f t="shared" ref="O27:O30" si="0">N27/$N$6</f>
+        <v>0.29411764705882354</v>
+      </c>
+    </row>
+    <row r="28" spans="12:23" x14ac:dyDescent="0.25">
+      <c r="L28">
+        <f>$L$9*N20</f>
+        <v>0</v>
+      </c>
+      <c r="M28" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="N28" s="26">
+        <f t="shared" ref="N28:N29" si="1">L28*(1-N11)</f>
+        <v>0</v>
+      </c>
+      <c r="O28" s="24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="12:23" x14ac:dyDescent="0.25">
+      <c r="L29" s="5">
+        <f>$L$9*N21</f>
+        <v>0</v>
+      </c>
+      <c r="M29" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="N29" s="27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O29" s="24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="12:23" x14ac:dyDescent="0.25">
+      <c r="L30">
+        <f>SUM(L26:L29)</f>
         <v>100</v>
       </c>
-      <c r="H8" s="7">
-        <f>VLOOKUP($C$2,Speciesdb!$B:$M,6)</f>
-        <v>100</v>
-      </c>
-      <c r="I8" s="7">
-        <f>VLOOKUP($C$2,Speciesdb!$B:$M,7)</f>
-        <v>0</v>
-      </c>
-      <c r="J8" s="7">
-        <f>VLOOKUP($C$2,Speciesdb!$B:$M,8)</f>
-        <v>0</v>
-      </c>
-      <c r="K8" s="7">
-        <f>VLOOKUP($C$2,Speciesdb!$B:$M,9)</f>
-        <v>0</v>
-      </c>
-      <c r="L8" s="8">
-        <f>VLOOKUP($C$2,Speciesdb!$B:$M,10)</f>
-        <v>100</v>
-      </c>
-      <c r="M8" t="str">
-        <f>VLOOKUP($C$2,Speciesdb!$B:$M,11)</f>
-        <v/>
-      </c>
-      <c r="N8" t="str">
-        <f>VLOOKUP($C$2,Speciesdb!$B:$M,12)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" t="s">
-        <v>27</v>
-      </c>
-      <c r="H12" t="s">
-        <v>28</v>
-      </c>
-      <c r="I12" t="s">
-        <v>29</v>
-      </c>
-      <c r="J12" t="s">
-        <v>13</v>
-      </c>
-      <c r="K12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="C13" s="15"/>
-      <c r="D13" t="str">
-        <f>VLOOKUP(B13,Attacksdb[[Name]:[Tooltip]],1)</f>
-        <v>Cold Reference</v>
-      </c>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
+      <c r="M30" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="N30" s="26">
+        <f>SUM(N26:N29)</f>
+        <v>70</v>
+      </c>
+      <c r="O30" s="24">
+        <f t="shared" si="0"/>
+        <v>0.29411764705882354</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="E6:L6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="C2:D2"/>
+  <mergeCells count="5">
+    <mergeCell ref="L18:L21"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="N3:O3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AF061547-00D3-413A-8119-2BCAB2B4E6C5}">
+          <x14:formula1>
+            <xm:f>Attacksdb!$B:$B</xm:f>
+          </x14:formula1>
+          <xm:sqref>M17</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DB79F550-D124-40A4-8E5C-B10F6DC20F25}">
+          <x14:formula1>
+            <xm:f>Speciesdb!$B:$B</xm:f>
+          </x14:formula1>
+          <xm:sqref>R10 K4:L4 N4:O4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1008,7 +1450,7 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1035,34 +1477,34 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
         <v>24</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>25</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>26</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>27</v>
-      </c>
-      <c r="G1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H1" t="s">
-        <v>29</v>
       </c>
       <c r="I1" t="s">
         <v>13</v>
       </c>
       <c r="J1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" t="s">
         <v>30</v>
-      </c>
-      <c r="K1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -1070,7 +1512,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1097,7 +1539,7 @@
         <v>15</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1105,7 +1547,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1132,7 +1574,7 @@
         <v>15</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1140,7 +1582,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -1167,7 +1609,7 @@
         <v>15</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1175,7 +1617,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -1202,7 +1644,7 @@
         <v>15</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1210,7 +1652,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C6">
         <v>1.2</v>
@@ -1231,13 +1673,13 @@
         <v>1</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>15</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1245,7 +1687,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C7">
         <v>0.6</v>
@@ -1266,13 +1708,13 @@
         <v>1</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1280,7 +1722,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -1301,13 +1743,13 @@
         <v>1</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1315,7 +1757,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1336,13 +1778,13 @@
         <v>1</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>15</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1350,7 +1792,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C10">
         <v>0.1</v>
@@ -1371,13 +1813,13 @@
         <v>1</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1385,34 +1827,34 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L11" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1420,7 +1862,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -1441,10 +1883,10 @@
         <v>1</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="K12">
         <v>11</v>
@@ -1458,7 +1900,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1479,10 +1921,10 @@
         <v>1</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K13">
         <v>12</v>
@@ -1496,7 +1938,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1517,7 +1959,7 @@
         <v>2</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>15</v>

</xml_diff>